<commit_message>
case and death col
</commit_message>
<xml_diff>
--- a/data/covid_data_dictionary_and_source.xlsx
+++ b/data/covid_data_dictionary_and_source.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kerrimac/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kerrimac/Desktop/covid_cases/east_lothian_covid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA6409A-E4FD-164C-BE3D-A98669860E9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87F0C19-BB7A-024F-9C7E-03203EF3D844}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="2000" windowWidth="28040" windowHeight="17440" xr2:uid="{36FCAAB3-C542-D145-B3E7-3909187E8B0C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
   <si>
     <t>Column</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Intermediate zone code 2011</t>
   </si>
   <si>
-    <t>Intermediate Zone labels</t>
-  </si>
-  <si>
     <t>IntZoneName</t>
   </si>
   <si>
@@ -223,13 +220,19 @@
   </si>
   <si>
     <t>Local Area Data Dictionary</t>
+  </si>
+  <si>
+    <t>Local area map</t>
+  </si>
+  <si>
+    <t>Intermediate Zones are a statistical geography that sit between Data Zones and council areas. Intermediate Zones are often used for the dissemination of statistics that are not suitable for release at the Data Zone level because of the sensitive nature of the statistic, or for reasons of reliability. Intermediate Zones were designed to meet constraints on population thresholds (2,500 - 6,000 household residents), to nest within council areas, and to be built up from aggregates of Data Zones. Intermediate Zones also represent a relatively stable geography that can be used to analyse change over time, with changes only occurring after a Census. Following Census 2011, there are now 1,279 Intermediate Zones covering the whole of Scotland.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -265,6 +268,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF292D33"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -287,7 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -296,6 +305,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -614,7 +624,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,6 +643,9 @@
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -848,7 +861,7 @@
     </row>
     <row r="24" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -877,7 +890,7 @@
       </c>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="23" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
@@ -887,19 +900,19 @@
       <c r="C27" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>46</v>
+      <c r="D27" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D28" s="3"/>
     </row>
@@ -911,7 +924,7 @@
         <v>8</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>10</v>
@@ -931,78 +944,77 @@
     </row>
     <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" display="https://www.opendata.nhs.scot/dataset/geography-codes-and-labels/resource/967937c4-8d67-4f39-974f-fd58c4acfda5" xr:uid="{0A93FC44-90AD-094B-A2C7-9B0DA697EBE6}"/>
-    <hyperlink ref="D27" r:id="rId2" display="https://www.opendata.nhs.scot/dataset/geography-codes-and-labels/resource/e3e885cc-2530-4b3c-bead-9eda9782264f" xr:uid="{E7B54494-C68D-574C-87C2-BCC011C301EA}"/>
-    <hyperlink ref="D29" r:id="rId3" display="https://www.opendata.nhs.scot/dataset/geography-codes-and-labels/resource/967937c4-8d67-4f39-974f-fd58c4acfda5" xr:uid="{C1120158-499E-2042-A50E-D20F307E04BC}"/>
-    <hyperlink ref="D32" r:id="rId4" display="https://www.opendata.nhs.scot/dataset/statistical-qualifiers/resource/b80f9af0-b115-4245-b591-fb22775226c4" xr:uid="{F32A371F-8039-B845-B383-5038BEA7E113}"/>
-    <hyperlink ref="D33" r:id="rId5" display="https://www.opendata.nhs.scot/dataset/population-estimates/resource/93df4c88-f74b-4630-abd8-459a19b12f47" xr:uid="{066255FE-2028-C34F-ABBC-4DC2150251B6}"/>
-    <hyperlink ref="D35" r:id="rId6" display="https://www.opendata.nhs.scot/dataset/statistical-qualifiers/resource/b80f9af0-b115-4245-b591-fb22775226c4" xr:uid="{ACC0F1D5-9C39-9148-A9F8-E9B1AA8D29A4}"/>
+    <hyperlink ref="D29" r:id="rId2" display="https://www.opendata.nhs.scot/dataset/geography-codes-and-labels/resource/967937c4-8d67-4f39-974f-fd58c4acfda5" xr:uid="{C1120158-499E-2042-A50E-D20F307E04BC}"/>
+    <hyperlink ref="D32" r:id="rId3" display="https://www.opendata.nhs.scot/dataset/statistical-qualifiers/resource/b80f9af0-b115-4245-b591-fb22775226c4" xr:uid="{F32A371F-8039-B845-B383-5038BEA7E113}"/>
+    <hyperlink ref="D33" r:id="rId4" display="https://www.opendata.nhs.scot/dataset/population-estimates/resource/93df4c88-f74b-4630-abd8-459a19b12f47" xr:uid="{066255FE-2028-C34F-ABBC-4DC2150251B6}"/>
+    <hyperlink ref="D35" r:id="rId5" display="https://www.opendata.nhs.scot/dataset/statistical-qualifiers/resource/b80f9af0-b115-4245-b591-fb22775226c4" xr:uid="{ACC0F1D5-9C39-9148-A9F8-E9B1AA8D29A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>